<commit_message>
Harmonized IRA data (closes #9)
</commit_message>
<xml_diff>
--- a/data/state-of-practice/data-extraction-ira.xlsx
+++ b/data/state-of-practice/data-extraction-ira.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juf\Workspace\BTH\Data Processing\b4c\data\state-of-practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7DEAA5-03E0-4285-AA69-E70221E467F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541934B3-BABF-4B7D-BE07-A64E33384511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-14805" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-14805" windowWidth="51840" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Studies" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="146">
   <si>
     <t>ID</t>
   </si>
@@ -234,18 +234,6 @@
     <t>Other</t>
   </si>
   <si>
-    <t>GUI test specification approach/technique</t>
-  </si>
-  <si>
-    <t>[Slang; JBehave]</t>
-  </si>
-  <si>
-    <t>efficiency</t>
-  </si>
-  <si>
-    <t>"time per test case was accumulated per participant and divided by the number of fully and correctly specified test cases to compute the average time per test case"</t>
-  </si>
-  <si>
     <t>GLMM</t>
   </si>
   <si>
@@ -253,9 +241,6 @@
   </si>
   <si>
     <t>Reachable</t>
-  </si>
-  <si>
-    <t>https://www.dropbox.com/scl/fo/jp4qi7xgiamxb5z45ggjl/ACK1ECptEMJ0UN0C3a4JqV8?rlkey=w4lnd0007dlzvv29mv7oifpe3&amp;e=1&amp;dl=0</t>
   </si>
   <si>
     <t>Tool version</t>
@@ -366,15 +351,6 @@
   </si>
   <si>
     <t>They call their method a "Linear Marginal Model" (LMM) ut describe it as "LMMs are linear models in which the residuals are not assumed to be independent of each other or have constant variance", which are GLMMs. The authors acknowledge a "training leakage effect", which sounds like the period threat.</t>
-  </si>
-  <si>
-    <t>BDD DSL</t>
-  </si>
-  <si>
-    <t>JBehave;Slang</t>
-  </si>
-  <si>
-    <t>time for correctly specified test case</t>
   </si>
   <si>
     <t>[Tab version; Panel version]</t>
@@ -841,17 +817,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -884,6 +849,17 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3385,7 +3361,7 @@
       </c>
       <c r="E65" s="5">
         <f ca="1">IF(C65, COUNTIF(Extraction!A:A, A65), "-")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F65" s="7" t="b">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("(COUNTIF(IMPORTRANGE(""https://docs.google.com/spreadsheets/d/1XUJGjtfB9SoW1rbohdkE9Z52MKac6AJzLHIsCSLTjGo/edit#gid=0"", ""Overlap!A2:A15""), A65)&gt;0)"),TRUE)</f>
@@ -3397,7 +3373,7 @@
       </c>
       <c r="H65" s="8">
         <f ca="1">IF(AND(C65,F65), COUNTIF(Overlap!A:A, A65), "-")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65" s="6"/>
     </row>
@@ -5897,13 +5873,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:S155"/>
+  <dimension ref="A1:S154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5924,61 +5900,61 @@
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="40" t="s">
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="39"/>
-      <c r="I1" s="37" t="s">
+      <c r="H1" s="50"/>
+      <c r="I1" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="37" t="s">
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="39"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="50"/>
       <c r="S1" s="2"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="40" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="39"/>
+      <c r="F2" s="50"/>
       <c r="G2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
       <c r="J2" s="34"/>
-      <c r="K2" s="37" t="s">
+      <c r="K2" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="37" t="s">
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="37" t="s">
+      <c r="P2" s="49"/>
+      <c r="Q2" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="39"/>
+      <c r="R2" s="50"/>
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -6001,10 +5977,10 @@
         <v>26</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>19</v>
@@ -6025,16 +6001,16 @@
         <v>30</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="P3" s="35" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="R3" s="36" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>15</v>
@@ -6191,7 +6167,7 @@
         <v>54</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N6" s="8" t="s">
         <v>54</v>
@@ -6262,52 +6238,52 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B8" s="8" t="str">
         <f ca="1">IF(ISBLANK(A8), "", VLOOKUP(A8, Studies!A:D, 4))</f>
-        <v>jfr</v>
+        <v>dfu</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G8" s="6">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" s="11"/>
+        <v>37</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="K8" s="5" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="P8" s="12" t="s">
-        <v>67</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="P8" s="9"/>
       <c r="Q8" s="5" t="s">
         <v>41</v>
       </c>
@@ -6316,11 +6292,11 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B9" s="8" t="str">
         <f ca="1">IF(ISBLANK(A9), "", VLOOKUP(A9, Studies!A:D, 4))</f>
-        <v>dfu</v>
+        <v>jfr</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>68</v>
@@ -6335,17 +6311,15 @@
         <v>71</v>
       </c>
       <c r="G9" s="6">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>72</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="J9" s="11"/>
       <c r="K9" s="5" t="s">
         <v>40</v>
       </c>
@@ -6353,75 +6327,81 @@
         <v>40</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="N9" s="8" t="s">
         <v>40</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P9" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="P9" s="12" t="s">
+        <v>73</v>
+      </c>
       <c r="Q9" s="5" t="s">
         <v>41</v>
       </c>
       <c r="R9" s="10"/>
-      <c r="S9" s="6"/>
+      <c r="S9" s="6" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="B10" s="8" t="str">
         <f ca="1">IF(ISBLANK(A10), "", VLOOKUP(A10, Studies!A:D, 4))</f>
         <v>jfr</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G10" s="6">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J10" s="11"/>
       <c r="K10" s="5" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N10" s="8" t="s">
         <v>40</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="P10" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="R10" s="10"/>
+        <v>79</v>
+      </c>
+      <c r="R10" s="13" t="s">
+        <v>80</v>
+      </c>
       <c r="S10" s="6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -6433,32 +6413,32 @@
         <v>jfr</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G11" s="6">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>36</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J11" s="11"/>
       <c r="K11" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>39</v>
@@ -6467,20 +6447,18 @@
         <v>40</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="P11" s="12" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="R11" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="S11" s="6" t="s">
-        <v>86</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="S11" s="6"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -6491,32 +6469,32 @@
         <v>jfr</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G12" s="6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>36</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J12" s="11"/>
       <c r="K12" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M12" s="5" t="s">
         <v>39</v>
@@ -6525,77 +6503,40 @@
         <v>40</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="P12" s="12" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="R12" s="13" t="s">
-        <v>85</v>
+        <v>79</v>
+      </c>
+      <c r="R12" s="14" t="s">
+        <v>80</v>
       </c>
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>116</v>
-      </c>
-      <c r="B13" s="8" t="str">
-        <f ca="1">IF(ISBLANK(A13), "", VLOOKUP(A13, Studies!A:D, 4))</f>
-        <v>jfr</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="G13" s="6">
-        <v>11</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>64</v>
-      </c>
+      <c r="A13" s="5"/>
+      <c r="B13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="5"/>
       <c r="J13" s="11"/>
-      <c r="K13" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="N13" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="P13" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q13" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="R13" s="14" t="s">
-        <v>85</v>
-      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="10"/>
       <c r="S13" s="6"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
       <c r="B14" s="8"/>
       <c r="D14" s="9"/>
       <c r="E14" s="6"/>
@@ -9274,25 +9215,6 @@
       <c r="R154" s="10"/>
       <c r="S154" s="6"/>
     </row>
-    <row r="155" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B155" s="8"/>
-      <c r="D155" s="9"/>
-      <c r="E155" s="6"/>
-      <c r="F155" s="10"/>
-      <c r="G155" s="6"/>
-      <c r="H155" s="8"/>
-      <c r="I155" s="5"/>
-      <c r="J155" s="11"/>
-      <c r="K155" s="5"/>
-      <c r="L155" s="5"/>
-      <c r="M155" s="5"/>
-      <c r="N155" s="8"/>
-      <c r="O155" s="5"/>
-      <c r="P155" s="9"/>
-      <c r="Q155" s="5"/>
-      <c r="R155" s="10"/>
-      <c r="S155" s="6"/>
-    </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="O2:P2"/>
@@ -9306,49 +9228,66 @@
     <mergeCell ref="K2:N2"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K4:N155" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K4:N154" xr:uid="{19612D46-DB6E-40E8-BEE4-2EEEE9D5D957}">
       <formula1>"Parameter,Stratification,Isolation,Acknowledged,Ignored"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B4:B155" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B4:B154" xr:uid="{EB1A602E-B098-496A-B27E-2626E502781F}">
       <formula1>"dfu,jfr"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="O4:O155 Q4:Q155" xr:uid="{00000000-0002-0000-0100-000004000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="Q4:Q154 O4:O154" xr:uid="{A6C322F2-1ADE-4DF5-9F55-4FC7BDAA010B}">
       <formula1>"Archived,Open Source,Reachable,Upon Request,Broken,Unavailable,Private,Proprietary"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="P5" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="R5" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="P8" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="P10" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="P11" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="R11" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="P12" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="R12" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="P13" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="R13" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="P9" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="P10" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="R10" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="P11" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="R11" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="P12" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="R12" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{073F4C58-C1A9-4492-9A7C-C5DB1635329B}">
           <x14:formula1>
             <xm:f>CategoriesMethod!$A$2:$A155</xm:f>
           </x14:formula1>
-          <xm:sqref>I4:I155</xm:sqref>
+          <xm:sqref>I4:I7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{D44CC31F-0E55-4D96-97AD-D292AD270879}">
+          <x14:formula1>
+            <xm:f>CategoriesMethod!$A$2:$A160</xm:f>
+          </x14:formula1>
+          <xm:sqref>I8:I154</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{1DAC8103-41B2-47F7-BF7A-58541B614BC0}">
           <x14:formula1>
             <xm:f>CategoriesTesttype!$A$2:$A155</xm:f>
           </x14:formula1>
-          <xm:sqref>J4:J155</xm:sqref>
+          <xm:sqref>J4:J7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{80AB2DD4-D39A-4F4A-A39A-019DD8450586}">
+          <x14:formula1>
+            <xm:f>CategoriesTesttype!$A$2:$A160</xm:f>
+          </x14:formula1>
+          <xm:sqref>J8:J154</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{EC2E614D-A2B8-4A85-88A3-A922BE03163F}">
           <x14:formula1>
             <xm:f>CategoriesSubjects!$A$2:$A155</xm:f>
           </x14:formula1>
-          <xm:sqref>H4:H155</xm:sqref>
+          <xm:sqref>H4:H7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{07BDD346-8D30-480D-95CC-A288506144DC}">
+          <x14:formula1>
+            <xm:f>CategoriesSubjects!$A$2:$A160</xm:f>
+          </x14:formula1>
+          <xm:sqref>H8:H154</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -9361,13 +9300,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:S153"/>
+  <dimension ref="A1:S152"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M31" sqref="M31"/>
+      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9388,67 +9327,67 @@
     <col min="19" max="19" width="50.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="40" t="s">
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="39"/>
-      <c r="I1" s="37" t="s">
+      <c r="H1" s="50"/>
+      <c r="I1" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="37" t="s">
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="39"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="50"/>
       <c r="S1" s="2"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="40" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="39"/>
+      <c r="F2" s="50"/>
       <c r="G2" s="2"/>
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
       <c r="J2" s="34"/>
-      <c r="K2" s="37" t="s">
+      <c r="K2" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="37" t="s">
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="37" t="s">
+      <c r="P2" s="49"/>
+      <c r="Q2" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="39"/>
+      <c r="R2" s="50"/>
       <c r="S2" s="2"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -9468,10 +9407,10 @@
         <v>26</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>19</v>
@@ -9492,16 +9431,16 @@
         <v>30</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="P3" s="35" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="R3" s="36" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>15</v>
@@ -9516,18 +9455,18 @@
         <v>jfr</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="G4" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="47" t="s">
         <v>35</v>
       </c>
       <c r="H4" s="8" t="s">
@@ -9560,27 +9499,27 @@
       </c>
       <c r="R4" s="10"/>
       <c r="S4" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="52.8" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>9</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G5" s="6">
         <v>105</v>
@@ -9620,7 +9559,7 @@
       </c>
       <c r="S5" s="6"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>14</v>
       </c>
@@ -9629,16 +9568,16 @@
         <v>jfr</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>50</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G6" s="6">
         <v>21</v>
@@ -9673,10 +9612,10 @@
       </c>
       <c r="R6" s="10"/>
       <c r="S6" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>48</v>
       </c>
@@ -9685,16 +9624,16 @@
         <v>jfr</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G7" s="6">
         <v>18</v>
@@ -9703,7 +9642,7 @@
         <v>36</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J7" s="11"/>
       <c r="K7" s="5" t="s">
@@ -9727,92 +9666,90 @@
       </c>
       <c r="R7" s="10"/>
       <c r="S7" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>64</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>92</v>
+        <v>71</v>
+      </c>
+      <c r="B8" s="8" t="str">
+        <f ca="1">IF(ISBLANK(A8), "", IF(VLOOKUP(A8, Studies!A:D, 2)="jfr", "dfu", "jfr"))</f>
+        <v>jfr</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>106</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="F8" s="10"/>
       <c r="G8" s="6">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" s="11"/>
+        <v>37</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="K8" s="5" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="P8" s="12" t="s">
-        <v>67</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="P8" s="9"/>
       <c r="Q8" s="5" t="s">
         <v>41</v>
       </c>
       <c r="R8" s="10"/>
       <c r="S8" s="6"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
-        <v>71</v>
-      </c>
-      <c r="B9" s="8" t="str">
-        <f ca="1">IF(ISBLANK(A9), "", IF(VLOOKUP(A9, Studies!A:D, 2)="jfr", "dfu", "jfr"))</f>
-        <v>jfr</v>
+        <v>77</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="F9" s="10"/>
+        <v>103</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>104</v>
+      </c>
       <c r="G9" s="6">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J9" s="11" t="s">
         <v>72</v>
       </c>
+      <c r="J9" s="11"/>
       <c r="K9" s="5" t="s">
         <v>40</v>
       </c>
@@ -9820,15 +9757,17 @@
         <v>40</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="N9" s="8" t="s">
         <v>40</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P9" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="P9" s="12" t="s">
+        <v>73</v>
+      </c>
       <c r="Q9" s="5" t="s">
         <v>41</v>
       </c>
@@ -9836,222 +9775,189 @@
       <c r="S9" s="6"/>
     </row>
     <row r="10" spans="1:19" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="A10" s="37">
+        <v>116</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="G10" s="6">
-        <v>14</v>
-      </c>
-      <c r="H10" s="8" t="s">
+      <c r="F10" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="G10" s="37">
+        <v>18</v>
+      </c>
+      <c r="H10" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" s="40"/>
+      <c r="K10" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="L10" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="M10" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="N10" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="O10" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="P10" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q10" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="R10" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="S10" s="39"/>
+    </row>
+    <row r="11" spans="1:19" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="37">
+        <v>116</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="F11" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="G11" s="37">
+        <v>10</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" s="40"/>
+      <c r="K11" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="L11" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="M11" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="N11" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="O11" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="P11" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q11" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="R11" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="S11" s="39"/>
+    </row>
+    <row r="12" spans="1:19" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="37">
+        <v>116</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="J10" s="11"/>
-      <c r="K10" s="5" t="s">
+      <c r="F12" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="G12" s="37">
+        <v>11</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="J12" s="40"/>
+      <c r="K12" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="L12" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="M12" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="N12" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="L10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="N10" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="P10" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="R10" s="10"/>
-      <c r="S10" s="6"/>
-    </row>
-    <row r="11" spans="1:19" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="42">
-        <v>116</v>
-      </c>
-      <c r="B11" s="43" t="s">
-        <v>92</v>
-      </c>
-      <c r="C11" s="44" t="s">
-        <v>113</v>
-      </c>
-      <c r="D11" s="45" t="s">
-        <v>114</v>
-      </c>
-      <c r="E11" s="44" t="s">
-        <v>82</v>
-      </c>
-      <c r="F11" s="46" t="s">
-        <v>115</v>
-      </c>
-      <c r="G11" s="42">
-        <v>18</v>
-      </c>
-      <c r="H11" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="J11" s="45"/>
-      <c r="K11" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="L11" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="M11" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="N11" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="O11" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="P11" s="50" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q11" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="R11" s="51" t="s">
-        <v>116</v>
-      </c>
-      <c r="S11" s="44"/>
-    </row>
-    <row r="12" spans="1:19" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="42">
-        <v>116</v>
-      </c>
-      <c r="B12" s="43" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" s="44" t="s">
-        <v>113</v>
-      </c>
-      <c r="D12" s="45" t="s">
-        <v>114</v>
-      </c>
-      <c r="E12" s="44" t="s">
-        <v>82</v>
-      </c>
-      <c r="F12" s="46" t="s">
-        <v>115</v>
-      </c>
-      <c r="G12" s="42">
-        <v>10</v>
-      </c>
-      <c r="H12" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="I12" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="J12" s="45"/>
-      <c r="K12" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="L12" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="M12" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="N12" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="O12" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="P12" s="50" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q12" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="R12" s="51" t="s">
-        <v>116</v>
-      </c>
-      <c r="S12" s="44"/>
-    </row>
-    <row r="13" spans="1:19" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="42">
-        <v>116</v>
-      </c>
-      <c r="B13" s="43" t="s">
-        <v>92</v>
-      </c>
-      <c r="C13" s="44" t="s">
-        <v>113</v>
-      </c>
-      <c r="D13" s="45" t="s">
-        <v>114</v>
-      </c>
-      <c r="E13" s="44" t="s">
-        <v>82</v>
-      </c>
-      <c r="F13" s="46" t="s">
-        <v>115</v>
-      </c>
-      <c r="G13" s="42">
-        <v>11</v>
-      </c>
-      <c r="H13" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="I13" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="J13" s="45"/>
-      <c r="K13" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="L13" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="M13" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="N13" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="O13" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="P13" s="50" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q13" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="R13" s="51" t="s">
-        <v>116</v>
-      </c>
-      <c r="S13" s="44"/>
+      <c r="O12" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="P12" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q12" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="R12" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="S12" s="39"/>
+    </row>
+    <row r="13" spans="1:19" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="6"/>
     </row>
     <row r="14" spans="1:19" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B14" s="8"/>
@@ -12833,26 +12739,6 @@
       <c r="R152" s="10"/>
       <c r="S152" s="6"/>
     </row>
-    <row r="153" spans="2:19" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B153" s="8"/>
-      <c r="C153" s="6"/>
-      <c r="D153" s="9"/>
-      <c r="E153" s="6"/>
-      <c r="F153" s="10"/>
-      <c r="G153" s="6"/>
-      <c r="H153" s="8"/>
-      <c r="I153" s="5"/>
-      <c r="J153" s="11"/>
-      <c r="K153" s="5"/>
-      <c r="L153" s="5"/>
-      <c r="M153" s="5"/>
-      <c r="N153" s="8"/>
-      <c r="O153" s="5"/>
-      <c r="P153" s="9"/>
-      <c r="Q153" s="5"/>
-      <c r="R153" s="10"/>
-      <c r="S153" s="6"/>
-    </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="K2:N2"/>
@@ -12866,49 +12752,66 @@
     <mergeCell ref="Q2:R2"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K4:N10 K14:N153" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K13:N152 K4:N9" xr:uid="{55F6383A-0435-48B9-82D1-7A71BED1C8E8}">
       <formula1>"Parameter,Stratification,Isolation,Acknowledged,Ignored"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B4:B10 B14:B153" xr:uid="{00000000-0002-0000-0200-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B13:B152 B4:B9" xr:uid="{1EAA4867-592E-4C8D-A495-F9B5EA829E07}">
       <formula1>"jfr,dju"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="Q14:Q153 Q4:Q10 O4:O10 O14:O153" xr:uid="{00000000-0002-0000-0200-000004000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="Q13:Q152 O13:O152 O4:O9 Q4:Q9" xr:uid="{715A81E0-7679-436E-B3CA-3B4E3A80E662}">
       <formula1>"Archived,Open Source,Reachable,Upon Request,Broken,Unavailable,Private,Proprietary"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="P5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
     <hyperlink ref="R5" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="P8" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="P10" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="P11" r:id="rId5" xr:uid="{1F705E6F-0CA7-4E95-88B0-906F755E9970}"/>
-    <hyperlink ref="R11" r:id="rId6" xr:uid="{7C29CFA5-2B26-49A5-89F7-E7E213727DBC}"/>
-    <hyperlink ref="P12" r:id="rId7" xr:uid="{06584F44-8A0F-4FA0-A7CB-4E61D2513A81}"/>
-    <hyperlink ref="R12" r:id="rId8" xr:uid="{DD662DB1-F711-44C3-980D-CDFCC4228A07}"/>
-    <hyperlink ref="P13" r:id="rId9" xr:uid="{B60DD6E6-A92A-4E21-A963-C6263F6ACB57}"/>
-    <hyperlink ref="R13" r:id="rId10" xr:uid="{18C88E5A-FA6A-42AC-9EA3-60248BE82BB5}"/>
+    <hyperlink ref="P9" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="P10" r:id="rId4" xr:uid="{1F705E6F-0CA7-4E95-88B0-906F755E9970}"/>
+    <hyperlink ref="R10" r:id="rId5" xr:uid="{7C29CFA5-2B26-49A5-89F7-E7E213727DBC}"/>
+    <hyperlink ref="P11" r:id="rId6" xr:uid="{06584F44-8A0F-4FA0-A7CB-4E61D2513A81}"/>
+    <hyperlink ref="R11" r:id="rId7" xr:uid="{DD662DB1-F711-44C3-980D-CDFCC4228A07}"/>
+    <hyperlink ref="P12" r:id="rId8" xr:uid="{B60DD6E6-A92A-4E21-A963-C6263F6ACB57}"/>
+    <hyperlink ref="R12" r:id="rId9" xr:uid="{18C88E5A-FA6A-42AC-9EA3-60248BE82BB5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{2B70BF8B-5E01-47CB-9162-FA992D914D6D}">
+          <x14:formula1>
+            <xm:f>CategoriesMethod!$A$2:$A158</xm:f>
+          </x14:formula1>
+          <xm:sqref>I13:I152 I8:I9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{67364343-0C37-4F15-BF25-F3FFB0394B92}">
+          <x14:formula1>
+            <xm:f>CategoriesTesttype!$A$2:$A158</xm:f>
+          </x14:formula1>
+          <xm:sqref>J13:J152 J8:J9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{BA3F6FE9-EBB2-469A-9A33-10767DDBC5D5}">
+          <x14:formula1>
+            <xm:f>CategoriesSubjects!$A$2:$A158</xm:f>
+          </x14:formula1>
+          <xm:sqref>H13:H152 H8:H9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{10C920C0-13D7-4795-AD0F-F55F3727E73C}">
           <x14:formula1>
             <xm:f>CategoriesMethod!$A$2:$A153</xm:f>
           </x14:formula1>
-          <xm:sqref>I4:I10 I14:I153</xm:sqref>
+          <xm:sqref>I4:I7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{31790532-A3DC-4C2B-9CB6-A77591A66FA5}">
           <x14:formula1>
             <xm:f>CategoriesTesttype!$A$2:$A153</xm:f>
           </x14:formula1>
-          <xm:sqref>J4:J10 J14:J153</xm:sqref>
+          <xm:sqref>J4:J7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{682CB3F6-8F2D-4B32-9E94-1E068FF624EC}">
           <x14:formula1>
             <xm:f>CategoriesSubjects!$A$2:$A153</xm:f>
           </x14:formula1>
-          <xm:sqref>H4:H10 H14:H153</xm:sqref>
+          <xm:sqref>H4:H7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -12933,78 +12836,78 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="41" t="s">
-        <v>121</v>
-      </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="41" t="s">
-        <v>122</v>
-      </c>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
+        <v>110</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="52" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="16" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="J2" s="15" t="s">
         <v>5</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="M2" s="15" t="s">
         <v>5</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C3" s="20">
         <f ca="1">SUMPRODUCT((Studies!D:D = A3) * (Studies!C:C = TRUE))</f>
@@ -13020,7 +12923,7 @@
       </c>
       <c r="F3" s="20">
         <f ca="1">SUMPRODUCT((Studies!D:D = A3) * (Studies!C:C = TRUE) * (Studies!E:E &gt; 0))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G3" s="21">
         <f ca="1">SUMPRODUCT((Studies!G:G = A3) * (Studies!C:C = TRUE) * (Studies!H:H &gt; 0))</f>
@@ -13028,11 +12931,11 @@
       </c>
       <c r="H3" s="22">
         <f t="shared" ref="H3:H5" ca="1" si="1">F3+G3</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I3" s="23">
         <f t="shared" ref="I3:K3" ca="1" si="2">F3/C3</f>
-        <v>0.14285714285714285</v>
+        <v>0.10714285714285714</v>
       </c>
       <c r="J3" s="24">
         <f t="shared" ca="1" si="2"/>
@@ -13040,11 +12943,11 @@
       </c>
       <c r="K3" s="25">
         <f t="shared" ca="1" si="2"/>
-        <v>0.25</v>
+        <v>0.21875</v>
       </c>
       <c r="L3" s="20">
         <f t="shared" ref="L3:M3" ca="1" si="3">C3-F3</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M3" s="21">
         <f t="shared" ca="1" si="3"/>
@@ -13052,15 +12955,15 @@
       </c>
       <c r="N3" s="22">
         <f t="shared" ref="N3:N5" ca="1" si="4">L3+M3</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C4" s="20">
         <f ca="1">SUMPRODUCT((Studies!D:D = A4) * (Studies!C:C = TRUE))</f>
@@ -13080,11 +12983,11 @@
       </c>
       <c r="G4" s="21">
         <f ca="1">SUMPRODUCT((Studies!G:G = A4) * (Studies!C:C = TRUE) * (Studies!H:H &gt; 0))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H4" s="22">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I4" s="23">
         <f t="shared" ref="I4:K4" ca="1" si="5">F4/C4</f>
@@ -13092,11 +12995,11 @@
       </c>
       <c r="J4" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="K4" s="25">
         <f t="shared" ca="1" si="5"/>
-        <v>0.23529411764705882</v>
+        <v>0.20588235294117646</v>
       </c>
       <c r="L4" s="20">
         <f t="shared" ref="L4:M4" ca="1" si="6">C4-F4</f>
@@ -13104,11 +13007,11 @@
       </c>
       <c r="M4" s="21">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4" s="22">
         <f t="shared" ca="1" si="4"/>
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -13128,39 +13031,39 @@
       </c>
       <c r="F5" s="27">
         <f t="shared" ref="F5:G5" ca="1" si="8">SUM(F3:F4)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" s="28">
         <f t="shared" ca="1" si="8"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H5" s="29">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I5" s="30">
         <f t="shared" ref="I5:M5" ca="1" si="9">SUM(I3:I4)</f>
-        <v>0.27619047619047621</v>
+        <v>0.24047619047619045</v>
       </c>
       <c r="J5" s="31">
         <f t="shared" ca="1" si="9"/>
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="K5" s="32">
         <f t="shared" ca="1" si="9"/>
-        <v>0.48529411764705882</v>
+        <v>0.42463235294117646</v>
       </c>
       <c r="L5" s="27">
         <f t="shared" ca="1" si="9"/>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M5" s="28">
         <f t="shared" ca="1" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="29">
         <f t="shared" ca="1" si="4"/>
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -13242,10 +13145,10 @@
         <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -13260,7 +13163,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="5">
@@ -13280,7 +13183,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="5">
@@ -13323,16 +13226,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -13340,10 +13243,10 @@
         <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D2" s="5">
         <f>COUNTIF(Extraction!I:I, A2)</f>
@@ -13352,13 +13255,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D3" s="5">
         <f>COUNTIF(Extraction!I:I, A3)</f>
@@ -13367,28 +13270,28 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D4" s="5">
         <f>COUNTIF(Extraction!I:I, A4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D5" s="5">
         <f>COUNTIF(Extraction!I:I, A5)</f>
@@ -13401,7 +13304,7 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="6" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D6" s="5">
         <f>COUNTIF(Extraction!I:I, A6)</f>
@@ -13410,11 +13313,11 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="6" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D7" s="5">
         <f>COUNTIF(Extraction!I:I, A7)</f>
@@ -13456,18 +13359,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="5">
@@ -13477,7 +13380,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="5">
@@ -13507,7 +13410,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="5">

</xml_diff>